<commit_message>
Formatted the tables nicely. Trying to determine best way to export
</commit_message>
<xml_diff>
--- a/Decoupling/tableTemplate.xlsx
+++ b/Decoupling/tableTemplate.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ensxvd_mail_missouri_edu/Documents/FAPRI/MarketResearch/Decoupling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{6B02D98A-47BB-48FE-9A6C-319F8F18CA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3CAED44B-AF81-412B-8812-98C8D477B31F}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="114_{E64F9D53-B268-47B0-A535-E4631D69459A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93678C12-E661-4581-A03E-C73C32FB5122}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2C021E1E-A2C6-47E3-A832-2AA0528880E4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2C021E1E-A2C6-47E3-A832-2AA0528880E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>Fixed direct payment (contract payment)</t>
   </si>
   <si>
     <t>Percent change in output / per-unit payment dollar or euro</t>
@@ -130,12 +128,51 @@
   <si>
     <t>V23</t>
   </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>US National</t>
+  </si>
+  <si>
+    <t>Corn Belt</t>
+  </si>
+  <si>
+    <t>Simulation or Theory</t>
+  </si>
+  <si>
+    <t>All &amp; Own Effect</t>
+  </si>
+  <si>
+    <t>Methods &amp; Own Effect</t>
+  </si>
+  <si>
+    <t>Region &amp; Own Effect</t>
+  </si>
+  <si>
+    <t>Nature of Effect</t>
+  </si>
+  <si>
+    <t>Cross-Effect</t>
+  </si>
+  <si>
+    <t>All Crops</t>
+  </si>
+  <si>
+    <t>One Crop</t>
+  </si>
+  <si>
+    <t>Est., Panel or Survey Data</t>
+  </si>
+  <si>
+    <t>Est., Market Data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +206,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,17 +240,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,16 +598,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFF912D-FCE7-43F6-89BC-50A1CD9B0337}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="4.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="4.36328125" style="1" customWidth="1"/>
     <col min="10" max="13" width="4.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="4.36328125" style="1" customWidth="1"/>
@@ -544,170 +622,170 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
@@ -734,7 +812,7 @@
     </row>
     <row r="5" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -759,7 +837,7 @@
     </row>
     <row r="6" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -911,7 +989,7 @@
     </row>
     <row r="9" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -936,7 +1014,7 @@
     </row>
     <row r="10" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1088,7 +1166,7 @@
     </row>
     <row r="13" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1175,22 +1253,22 @@
     </row>
     <row r="15" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15"/>
@@ -1234,7 +1312,7 @@
     </row>
     <row r="17" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -1259,7 +1337,7 @@
     </row>
     <row r="18" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1411,7 +1489,7 @@
     </row>
     <row r="21" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21"/>
       <c r="E21"/>
@@ -1436,7 +1514,7 @@
     </row>
     <row r="22" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1588,7 +1666,7 @@
     </row>
     <row r="25" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1682,22 +1760,2789 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CFEF19-65F2-4B7A-B20C-D8F1581CCEE7}">
+  <dimension ref="A1:U70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="44.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
+        <v>1</v>
+      </c>
+      <c r="P5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>1</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1</v>
+      </c>
+      <c r="T5" s="8">
+        <v>1</v>
+      </c>
+      <c r="U5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8">
+        <v>1</v>
+      </c>
+      <c r="P6" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>1</v>
+      </c>
+      <c r="R6" s="8">
+        <v>1</v>
+      </c>
+      <c r="S6" s="8">
+        <v>1</v>
+      </c>
+      <c r="T6" s="8">
+        <v>1</v>
+      </c>
+      <c r="U6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="U7" s="9"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="8">
+        <v>1</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>1</v>
+      </c>
+      <c r="R9" s="8">
+        <v>1</v>
+      </c>
+      <c r="S9" s="8">
+        <v>1</v>
+      </c>
+      <c r="T9" s="8">
+        <v>1</v>
+      </c>
+      <c r="U9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="U10" s="9"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8">
+        <v>1</v>
+      </c>
+      <c r="P11" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
+      <c r="R11" s="8">
+        <v>1</v>
+      </c>
+      <c r="S11" s="8">
+        <v>1</v>
+      </c>
+      <c r="T11" s="8">
+        <v>1</v>
+      </c>
+      <c r="U11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+      <c r="L12" s="8">
+        <v>1</v>
+      </c>
+      <c r="M12" s="8">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
+        <v>1</v>
+      </c>
+      <c r="P12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>1</v>
+      </c>
+      <c r="R12" s="8">
+        <v>1</v>
+      </c>
+      <c r="S12" s="8">
+        <v>1</v>
+      </c>
+      <c r="T12" s="8">
+        <v>1</v>
+      </c>
+      <c r="U12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="U13" s="9"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="U14" s="9"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1</v>
+      </c>
+      <c r="M15" s="8">
+        <v>1</v>
+      </c>
+      <c r="N15" s="8">
+        <v>1</v>
+      </c>
+      <c r="O15" s="8">
+        <v>1</v>
+      </c>
+      <c r="P15" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>1</v>
+      </c>
+      <c r="R15" s="8">
+        <v>1</v>
+      </c>
+      <c r="S15" s="8">
+        <v>1</v>
+      </c>
+      <c r="T15" s="8">
+        <v>1</v>
+      </c>
+      <c r="U15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1</v>
+      </c>
+      <c r="J16" s="8">
+        <v>1</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8">
+        <v>1</v>
+      </c>
+      <c r="N16" s="8">
+        <v>1</v>
+      </c>
+      <c r="O16" s="8">
+        <v>1</v>
+      </c>
+      <c r="P16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1</v>
+      </c>
+      <c r="R16" s="8">
+        <v>1</v>
+      </c>
+      <c r="S16" s="8">
+        <v>1</v>
+      </c>
+      <c r="T16" s="8">
+        <v>1</v>
+      </c>
+      <c r="U16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="U17" s="9"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18" s="8">
+        <v>1</v>
+      </c>
+      <c r="N18" s="8">
+        <v>1</v>
+      </c>
+      <c r="O18" s="8">
+        <v>1</v>
+      </c>
+      <c r="P18" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>1</v>
+      </c>
+      <c r="R18" s="8">
+        <v>1</v>
+      </c>
+      <c r="S18" s="8">
+        <v>1</v>
+      </c>
+      <c r="T18" s="8">
+        <v>1</v>
+      </c>
+      <c r="U18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1</v>
+      </c>
+      <c r="L19" s="8">
+        <v>1</v>
+      </c>
+      <c r="M19" s="8">
+        <v>1</v>
+      </c>
+      <c r="N19" s="8">
+        <v>1</v>
+      </c>
+      <c r="O19" s="8">
+        <v>1</v>
+      </c>
+      <c r="P19" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>1</v>
+      </c>
+      <c r="R19" s="8">
+        <v>1</v>
+      </c>
+      <c r="S19" s="8">
+        <v>1</v>
+      </c>
+      <c r="T19" s="8">
+        <v>1</v>
+      </c>
+      <c r="U19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1</v>
+      </c>
+      <c r="I21" s="8">
+        <v>1</v>
+      </c>
+      <c r="J21" s="8">
+        <v>1</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+      <c r="M21" s="8">
+        <v>1</v>
+      </c>
+      <c r="N21" s="8">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8">
+        <v>1</v>
+      </c>
+      <c r="P21" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>1</v>
+      </c>
+      <c r="R21" s="8">
+        <v>1</v>
+      </c>
+      <c r="S21" s="8">
+        <v>1</v>
+      </c>
+      <c r="T21" s="8">
+        <v>1</v>
+      </c>
+      <c r="U21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1</v>
+      </c>
+      <c r="J22" s="8">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8">
+        <v>1</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8">
+        <v>1</v>
+      </c>
+      <c r="N22" s="8">
+        <v>1</v>
+      </c>
+      <c r="O22" s="8">
+        <v>1</v>
+      </c>
+      <c r="P22" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>1</v>
+      </c>
+      <c r="R22" s="8">
+        <v>1</v>
+      </c>
+      <c r="S22" s="8">
+        <v>1</v>
+      </c>
+      <c r="T22" s="8">
+        <v>1</v>
+      </c>
+      <c r="U22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1</v>
+      </c>
+      <c r="I24" s="8">
+        <v>1</v>
+      </c>
+      <c r="J24" s="8">
+        <v>1</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+      <c r="M24" s="8">
+        <v>1</v>
+      </c>
+      <c r="N24" s="8">
+        <v>1</v>
+      </c>
+      <c r="O24" s="8">
+        <v>1</v>
+      </c>
+      <c r="P24" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>1</v>
+      </c>
+      <c r="R24" s="8">
+        <v>1</v>
+      </c>
+      <c r="S24" s="8">
+        <v>1</v>
+      </c>
+      <c r="T24" s="8">
+        <v>1</v>
+      </c>
+      <c r="U24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8">
+        <v>1</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8">
+        <v>1</v>
+      </c>
+      <c r="J25" s="8">
+        <v>1</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1</v>
+      </c>
+      <c r="L25" s="8">
+        <v>1</v>
+      </c>
+      <c r="M25" s="8">
+        <v>1</v>
+      </c>
+      <c r="N25" s="8">
+        <v>1</v>
+      </c>
+      <c r="O25" s="8">
+        <v>1</v>
+      </c>
+      <c r="P25" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>1</v>
+      </c>
+      <c r="R25" s="8">
+        <v>1</v>
+      </c>
+      <c r="S25" s="8">
+        <v>1</v>
+      </c>
+      <c r="T25" s="8">
+        <v>1</v>
+      </c>
+      <c r="U25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="U26" s="9"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8">
+        <v>1</v>
+      </c>
+      <c r="J28" s="8">
+        <v>1</v>
+      </c>
+      <c r="K28" s="8">
+        <v>1</v>
+      </c>
+      <c r="L28" s="8">
+        <v>1</v>
+      </c>
+      <c r="M28" s="8">
+        <v>1</v>
+      </c>
+      <c r="N28" s="8">
+        <v>1</v>
+      </c>
+      <c r="O28" s="8">
+        <v>1</v>
+      </c>
+      <c r="P28" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>1</v>
+      </c>
+      <c r="R28" s="8">
+        <v>1</v>
+      </c>
+      <c r="S28" s="8">
+        <v>1</v>
+      </c>
+      <c r="T28" s="8">
+        <v>1</v>
+      </c>
+      <c r="U28" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>1</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>1</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" s="8">
+        <v>1</v>
+      </c>
+      <c r="J29" s="8">
+        <v>1</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1</v>
+      </c>
+      <c r="N29" s="8">
+        <v>1</v>
+      </c>
+      <c r="O29" s="8">
+        <v>1</v>
+      </c>
+      <c r="P29" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>1</v>
+      </c>
+      <c r="R29" s="8">
+        <v>1</v>
+      </c>
+      <c r="S29" s="8">
+        <v>1</v>
+      </c>
+      <c r="T29" s="8">
+        <v>1</v>
+      </c>
+      <c r="U29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="U30" s="9"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>1</v>
+      </c>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8">
+        <v>1</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
+      </c>
+      <c r="I31" s="8">
+        <v>1</v>
+      </c>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
+      <c r="L31" s="8">
+        <v>1</v>
+      </c>
+      <c r="M31" s="8">
+        <v>1</v>
+      </c>
+      <c r="N31" s="8">
+        <v>1</v>
+      </c>
+      <c r="O31" s="8">
+        <v>1</v>
+      </c>
+      <c r="P31" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>1</v>
+      </c>
+      <c r="R31" s="8">
+        <v>1</v>
+      </c>
+      <c r="S31" s="8">
+        <v>1</v>
+      </c>
+      <c r="T31" s="8">
+        <v>1</v>
+      </c>
+      <c r="U31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1</v>
+      </c>
+      <c r="J32" s="8">
+        <v>1</v>
+      </c>
+      <c r="K32" s="8">
+        <v>1</v>
+      </c>
+      <c r="L32" s="8">
+        <v>1</v>
+      </c>
+      <c r="M32" s="8">
+        <v>1</v>
+      </c>
+      <c r="N32" s="8">
+        <v>1</v>
+      </c>
+      <c r="O32" s="8">
+        <v>1</v>
+      </c>
+      <c r="P32" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>1</v>
+      </c>
+      <c r="R32" s="8">
+        <v>1</v>
+      </c>
+      <c r="S32" s="8">
+        <v>1</v>
+      </c>
+      <c r="T32" s="8">
+        <v>1</v>
+      </c>
+      <c r="U32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D33" s="8"/>
+      <c r="F33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="U33" s="9"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8">
+        <v>1</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8">
+        <v>1</v>
+      </c>
+      <c r="J34" s="8">
+        <v>1</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1</v>
+      </c>
+      <c r="L34" s="8">
+        <v>1</v>
+      </c>
+      <c r="M34" s="8">
+        <v>1</v>
+      </c>
+      <c r="N34" s="8">
+        <v>1</v>
+      </c>
+      <c r="O34" s="8">
+        <v>1</v>
+      </c>
+      <c r="P34" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>1</v>
+      </c>
+      <c r="R34" s="8">
+        <v>1</v>
+      </c>
+      <c r="S34" s="8">
+        <v>1</v>
+      </c>
+      <c r="T34" s="8">
+        <v>1</v>
+      </c>
+      <c r="U34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8">
+        <v>1</v>
+      </c>
+      <c r="F35" s="8">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1</v>
+      </c>
+      <c r="I35" s="8">
+        <v>1</v>
+      </c>
+      <c r="J35" s="8">
+        <v>1</v>
+      </c>
+      <c r="K35" s="8">
+        <v>1</v>
+      </c>
+      <c r="L35" s="8">
+        <v>1</v>
+      </c>
+      <c r="M35" s="8">
+        <v>1</v>
+      </c>
+      <c r="N35" s="8">
+        <v>1</v>
+      </c>
+      <c r="O35" s="8">
+        <v>1</v>
+      </c>
+      <c r="P35" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>1</v>
+      </c>
+      <c r="R35" s="8">
+        <v>1</v>
+      </c>
+      <c r="S35" s="8">
+        <v>1</v>
+      </c>
+      <c r="T35" s="8">
+        <v>1</v>
+      </c>
+      <c r="U35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="U36" s="9"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="F38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="U38" s="9"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="8">
+        <v>1</v>
+      </c>
+      <c r="F39" s="8">
+        <v>1</v>
+      </c>
+      <c r="G39" s="8">
+        <v>1</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+      <c r="I39" s="8">
+        <v>1</v>
+      </c>
+      <c r="J39" s="8">
+        <v>1</v>
+      </c>
+      <c r="K39" s="8">
+        <v>1</v>
+      </c>
+      <c r="L39" s="8">
+        <v>1</v>
+      </c>
+      <c r="M39" s="8">
+        <v>1</v>
+      </c>
+      <c r="N39" s="8">
+        <v>1</v>
+      </c>
+      <c r="O39" s="8">
+        <v>1</v>
+      </c>
+      <c r="P39" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>1</v>
+      </c>
+      <c r="R39" s="8">
+        <v>1</v>
+      </c>
+      <c r="S39" s="8">
+        <v>1</v>
+      </c>
+      <c r="T39" s="8">
+        <v>1</v>
+      </c>
+      <c r="U39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="8">
+        <v>1</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1</v>
+      </c>
+      <c r="F40" s="8">
+        <v>1</v>
+      </c>
+      <c r="G40" s="8">
+        <v>1</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8">
+        <v>1</v>
+      </c>
+      <c r="J40" s="8">
+        <v>1</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1</v>
+      </c>
+      <c r="L40" s="8">
+        <v>1</v>
+      </c>
+      <c r="M40" s="8">
+        <v>1</v>
+      </c>
+      <c r="N40" s="8">
+        <v>1</v>
+      </c>
+      <c r="O40" s="8">
+        <v>1</v>
+      </c>
+      <c r="P40" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>1</v>
+      </c>
+      <c r="R40" s="8">
+        <v>1</v>
+      </c>
+      <c r="S40" s="8">
+        <v>1</v>
+      </c>
+      <c r="T40" s="8">
+        <v>1</v>
+      </c>
+      <c r="U40" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="U41" s="9"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1</v>
+      </c>
+      <c r="F42" s="8">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8">
+        <v>1</v>
+      </c>
+      <c r="H42" s="8">
+        <v>1</v>
+      </c>
+      <c r="I42" s="8">
+        <v>1</v>
+      </c>
+      <c r="J42" s="8">
+        <v>1</v>
+      </c>
+      <c r="K42" s="8">
+        <v>1</v>
+      </c>
+      <c r="L42" s="8">
+        <v>1</v>
+      </c>
+      <c r="M42" s="8">
+        <v>1</v>
+      </c>
+      <c r="N42" s="8">
+        <v>1</v>
+      </c>
+      <c r="O42" s="8">
+        <v>1</v>
+      </c>
+      <c r="P42" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>1</v>
+      </c>
+      <c r="R42" s="8">
+        <v>1</v>
+      </c>
+      <c r="S42" s="8">
+        <v>1</v>
+      </c>
+      <c r="T42" s="8">
+        <v>1</v>
+      </c>
+      <c r="U42" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="8">
+        <v>1</v>
+      </c>
+      <c r="E43" s="8">
+        <v>1</v>
+      </c>
+      <c r="F43" s="8">
+        <v>1</v>
+      </c>
+      <c r="G43" s="8">
+        <v>1</v>
+      </c>
+      <c r="H43" s="8">
+        <v>1</v>
+      </c>
+      <c r="I43" s="8">
+        <v>1</v>
+      </c>
+      <c r="J43" s="8">
+        <v>1</v>
+      </c>
+      <c r="K43" s="8">
+        <v>1</v>
+      </c>
+      <c r="L43" s="8">
+        <v>1</v>
+      </c>
+      <c r="M43" s="8">
+        <v>1</v>
+      </c>
+      <c r="N43" s="8">
+        <v>1</v>
+      </c>
+      <c r="O43" s="8">
+        <v>1</v>
+      </c>
+      <c r="P43" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>1</v>
+      </c>
+      <c r="R43" s="8">
+        <v>1</v>
+      </c>
+      <c r="S43" s="8">
+        <v>1</v>
+      </c>
+      <c r="T43" s="8">
+        <v>1</v>
+      </c>
+      <c r="U43" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="U44" s="9"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="8">
+        <v>1</v>
+      </c>
+      <c r="E45" s="8">
+        <v>1</v>
+      </c>
+      <c r="F45" s="8">
+        <v>1</v>
+      </c>
+      <c r="G45" s="8">
+        <v>1</v>
+      </c>
+      <c r="H45" s="8">
+        <v>1</v>
+      </c>
+      <c r="I45" s="8">
+        <v>1</v>
+      </c>
+      <c r="J45" s="8">
+        <v>1</v>
+      </c>
+      <c r="K45" s="8">
+        <v>1</v>
+      </c>
+      <c r="L45" s="8">
+        <v>1</v>
+      </c>
+      <c r="M45" s="8">
+        <v>1</v>
+      </c>
+      <c r="N45" s="8">
+        <v>1</v>
+      </c>
+      <c r="O45" s="8">
+        <v>1</v>
+      </c>
+      <c r="P45" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>1</v>
+      </c>
+      <c r="R45" s="8">
+        <v>1</v>
+      </c>
+      <c r="S45" s="8">
+        <v>1</v>
+      </c>
+      <c r="T45" s="8">
+        <v>1</v>
+      </c>
+      <c r="U45" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1</v>
+      </c>
+      <c r="E46" s="8">
+        <v>1</v>
+      </c>
+      <c r="F46" s="8">
+        <v>1</v>
+      </c>
+      <c r="G46" s="8">
+        <v>1</v>
+      </c>
+      <c r="H46" s="8">
+        <v>1</v>
+      </c>
+      <c r="I46" s="8">
+        <v>1</v>
+      </c>
+      <c r="J46" s="8">
+        <v>1</v>
+      </c>
+      <c r="K46" s="8">
+        <v>1</v>
+      </c>
+      <c r="L46" s="8">
+        <v>1</v>
+      </c>
+      <c r="M46" s="8">
+        <v>1</v>
+      </c>
+      <c r="N46" s="8">
+        <v>1</v>
+      </c>
+      <c r="O46" s="8">
+        <v>1</v>
+      </c>
+      <c r="P46" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>1</v>
+      </c>
+      <c r="R46" s="8">
+        <v>1</v>
+      </c>
+      <c r="S46" s="8">
+        <v>1</v>
+      </c>
+      <c r="T46" s="8">
+        <v>1</v>
+      </c>
+      <c r="U46" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D47" s="8"/>
+      <c r="F47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="U47" s="9"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="F48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="U48" s="9"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="8">
+        <v>1</v>
+      </c>
+      <c r="E49" s="8">
+        <v>1</v>
+      </c>
+      <c r="F49" s="8">
+        <v>1</v>
+      </c>
+      <c r="G49" s="8">
+        <v>1</v>
+      </c>
+      <c r="H49" s="8">
+        <v>1</v>
+      </c>
+      <c r="I49" s="8">
+        <v>1</v>
+      </c>
+      <c r="J49" s="8">
+        <v>1</v>
+      </c>
+      <c r="K49" s="8">
+        <v>1</v>
+      </c>
+      <c r="L49" s="8">
+        <v>1</v>
+      </c>
+      <c r="M49" s="8">
+        <v>1</v>
+      </c>
+      <c r="N49" s="8">
+        <v>1</v>
+      </c>
+      <c r="O49" s="8">
+        <v>1</v>
+      </c>
+      <c r="P49" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>1</v>
+      </c>
+      <c r="R49" s="8">
+        <v>1</v>
+      </c>
+      <c r="S49" s="8">
+        <v>1</v>
+      </c>
+      <c r="T49" s="8">
+        <v>1</v>
+      </c>
+      <c r="U49" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="8">
+        <v>1</v>
+      </c>
+      <c r="E50" s="8">
+        <v>1</v>
+      </c>
+      <c r="F50" s="8">
+        <v>1</v>
+      </c>
+      <c r="G50" s="8">
+        <v>1</v>
+      </c>
+      <c r="H50" s="8">
+        <v>1</v>
+      </c>
+      <c r="I50" s="8">
+        <v>1</v>
+      </c>
+      <c r="J50" s="8">
+        <v>1</v>
+      </c>
+      <c r="K50" s="8">
+        <v>1</v>
+      </c>
+      <c r="L50" s="8">
+        <v>1</v>
+      </c>
+      <c r="M50" s="8">
+        <v>1</v>
+      </c>
+      <c r="N50" s="8">
+        <v>1</v>
+      </c>
+      <c r="O50" s="8">
+        <v>1</v>
+      </c>
+      <c r="P50" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>1</v>
+      </c>
+      <c r="R50" s="8">
+        <v>1</v>
+      </c>
+      <c r="S50" s="8">
+        <v>1</v>
+      </c>
+      <c r="T50" s="8">
+        <v>1</v>
+      </c>
+      <c r="U50" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D51" s="8"/>
+      <c r="F51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="U51" s="9"/>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="8">
+        <v>1</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1</v>
+      </c>
+      <c r="F52" s="8">
+        <v>1</v>
+      </c>
+      <c r="G52" s="8">
+        <v>1</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1</v>
+      </c>
+      <c r="I52" s="8">
+        <v>1</v>
+      </c>
+      <c r="J52" s="8">
+        <v>1</v>
+      </c>
+      <c r="K52" s="8">
+        <v>1</v>
+      </c>
+      <c r="L52" s="8">
+        <v>1</v>
+      </c>
+      <c r="M52" s="8">
+        <v>1</v>
+      </c>
+      <c r="N52" s="8">
+        <v>1</v>
+      </c>
+      <c r="O52" s="8">
+        <v>1</v>
+      </c>
+      <c r="P52" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>1</v>
+      </c>
+      <c r="R52" s="8">
+        <v>1</v>
+      </c>
+      <c r="S52" s="8">
+        <v>1</v>
+      </c>
+      <c r="T52" s="8">
+        <v>1</v>
+      </c>
+      <c r="U52" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1</v>
+      </c>
+      <c r="F53" s="8">
+        <v>1</v>
+      </c>
+      <c r="G53" s="8">
+        <v>1</v>
+      </c>
+      <c r="H53" s="8">
+        <v>1</v>
+      </c>
+      <c r="I53" s="8">
+        <v>1</v>
+      </c>
+      <c r="J53" s="8">
+        <v>1</v>
+      </c>
+      <c r="K53" s="8">
+        <v>1</v>
+      </c>
+      <c r="L53" s="8">
+        <v>1</v>
+      </c>
+      <c r="M53" s="8">
+        <v>1</v>
+      </c>
+      <c r="N53" s="8">
+        <v>1</v>
+      </c>
+      <c r="O53" s="8">
+        <v>1</v>
+      </c>
+      <c r="P53" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>1</v>
+      </c>
+      <c r="R53" s="8">
+        <v>1</v>
+      </c>
+      <c r="S53" s="8">
+        <v>1</v>
+      </c>
+      <c r="T53" s="8">
+        <v>1</v>
+      </c>
+      <c r="U53" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D54" s="8"/>
+      <c r="F54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="U54" s="9"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="8">
+        <v>1</v>
+      </c>
+      <c r="E55" s="8">
+        <v>1</v>
+      </c>
+      <c r="F55" s="8">
+        <v>1</v>
+      </c>
+      <c r="G55" s="8">
+        <v>1</v>
+      </c>
+      <c r="H55" s="8">
+        <v>1</v>
+      </c>
+      <c r="I55" s="8">
+        <v>1</v>
+      </c>
+      <c r="J55" s="8">
+        <v>1</v>
+      </c>
+      <c r="K55" s="8">
+        <v>1</v>
+      </c>
+      <c r="L55" s="8">
+        <v>1</v>
+      </c>
+      <c r="M55" s="8">
+        <v>1</v>
+      </c>
+      <c r="N55" s="8">
+        <v>1</v>
+      </c>
+      <c r="O55" s="8">
+        <v>1</v>
+      </c>
+      <c r="P55" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>1</v>
+      </c>
+      <c r="R55" s="8">
+        <v>1</v>
+      </c>
+      <c r="S55" s="8">
+        <v>1</v>
+      </c>
+      <c r="T55" s="8">
+        <v>1</v>
+      </c>
+      <c r="U55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="8">
+        <v>1</v>
+      </c>
+      <c r="E56" s="8">
+        <v>1</v>
+      </c>
+      <c r="F56" s="8">
+        <v>1</v>
+      </c>
+      <c r="G56" s="8">
+        <v>1</v>
+      </c>
+      <c r="H56" s="8">
+        <v>1</v>
+      </c>
+      <c r="I56" s="8">
+        <v>1</v>
+      </c>
+      <c r="J56" s="8">
+        <v>1</v>
+      </c>
+      <c r="K56" s="8">
+        <v>1</v>
+      </c>
+      <c r="L56" s="8">
+        <v>1</v>
+      </c>
+      <c r="M56" s="8">
+        <v>1</v>
+      </c>
+      <c r="N56" s="8">
+        <v>1</v>
+      </c>
+      <c r="O56" s="8">
+        <v>1</v>
+      </c>
+      <c r="P56" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>1</v>
+      </c>
+      <c r="R56" s="8">
+        <v>1</v>
+      </c>
+      <c r="S56" s="8">
+        <v>1</v>
+      </c>
+      <c r="T56" s="8">
+        <v>1</v>
+      </c>
+      <c r="U56" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D57" s="8"/>
+      <c r="F57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="R57" s="9"/>
+      <c r="U57" s="9"/>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="8">
+        <v>1</v>
+      </c>
+      <c r="E58" s="8">
+        <v>1</v>
+      </c>
+      <c r="F58" s="8">
+        <v>1</v>
+      </c>
+      <c r="G58" s="8">
+        <v>1</v>
+      </c>
+      <c r="H58" s="8">
+        <v>1</v>
+      </c>
+      <c r="I58" s="8">
+        <v>1</v>
+      </c>
+      <c r="J58" s="8">
+        <v>1</v>
+      </c>
+      <c r="K58" s="8">
+        <v>1</v>
+      </c>
+      <c r="L58" s="8">
+        <v>1</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="8">
+        <v>1</v>
+      </c>
+      <c r="O58" s="8">
+        <v>1</v>
+      </c>
+      <c r="P58" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="8">
+        <v>1</v>
+      </c>
+      <c r="R58" s="8">
+        <v>1</v>
+      </c>
+      <c r="S58" s="8">
+        <v>1</v>
+      </c>
+      <c r="T58" s="8">
+        <v>1</v>
+      </c>
+      <c r="U58" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D59" s="8">
+        <v>1</v>
+      </c>
+      <c r="E59" s="8">
+        <v>1</v>
+      </c>
+      <c r="F59" s="8">
+        <v>1</v>
+      </c>
+      <c r="G59" s="8">
+        <v>1</v>
+      </c>
+      <c r="H59" s="8">
+        <v>1</v>
+      </c>
+      <c r="I59" s="8">
+        <v>1</v>
+      </c>
+      <c r="J59" s="8">
+        <v>1</v>
+      </c>
+      <c r="K59" s="8">
+        <v>1</v>
+      </c>
+      <c r="L59" s="8">
+        <v>1</v>
+      </c>
+      <c r="M59" s="8">
+        <v>1</v>
+      </c>
+      <c r="N59" s="8">
+        <v>1</v>
+      </c>
+      <c r="O59" s="8">
+        <v>1</v>
+      </c>
+      <c r="P59" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="8">
+        <v>1</v>
+      </c>
+      <c r="R59" s="8">
+        <v>1</v>
+      </c>
+      <c r="S59" s="8">
+        <v>1</v>
+      </c>
+      <c r="T59" s="8">
+        <v>1</v>
+      </c>
+      <c r="U59" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D60" s="8"/>
+      <c r="F60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="R60" s="9"/>
+      <c r="U60" s="9"/>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="F61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="R61" s="9"/>
+      <c r="U61" s="9"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="8">
+        <v>1</v>
+      </c>
+      <c r="E62" s="8">
+        <v>1</v>
+      </c>
+      <c r="F62" s="8">
+        <v>1</v>
+      </c>
+      <c r="G62" s="8">
+        <v>1</v>
+      </c>
+      <c r="H62" s="8">
+        <v>1</v>
+      </c>
+      <c r="I62" s="8">
+        <v>1</v>
+      </c>
+      <c r="J62" s="8">
+        <v>1</v>
+      </c>
+      <c r="K62" s="8">
+        <v>1</v>
+      </c>
+      <c r="L62" s="8">
+        <v>1</v>
+      </c>
+      <c r="M62" s="8">
+        <v>1</v>
+      </c>
+      <c r="N62" s="8">
+        <v>1</v>
+      </c>
+      <c r="O62" s="8">
+        <v>1</v>
+      </c>
+      <c r="P62" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="8">
+        <v>1</v>
+      </c>
+      <c r="R62" s="8">
+        <v>1</v>
+      </c>
+      <c r="S62" s="8">
+        <v>1</v>
+      </c>
+      <c r="T62" s="8">
+        <v>1</v>
+      </c>
+      <c r="U62" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="8">
+        <v>1</v>
+      </c>
+      <c r="E63" s="8">
+        <v>1</v>
+      </c>
+      <c r="F63" s="8">
+        <v>1</v>
+      </c>
+      <c r="G63" s="8">
+        <v>1</v>
+      </c>
+      <c r="H63" s="8">
+        <v>1</v>
+      </c>
+      <c r="I63" s="8">
+        <v>1</v>
+      </c>
+      <c r="J63" s="8">
+        <v>1</v>
+      </c>
+      <c r="K63" s="8">
+        <v>1</v>
+      </c>
+      <c r="L63" s="8">
+        <v>1</v>
+      </c>
+      <c r="M63" s="8">
+        <v>1</v>
+      </c>
+      <c r="N63" s="8">
+        <v>1</v>
+      </c>
+      <c r="O63" s="8">
+        <v>1</v>
+      </c>
+      <c r="P63" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="8">
+        <v>1</v>
+      </c>
+      <c r="R63" s="8">
+        <v>1</v>
+      </c>
+      <c r="S63" s="8">
+        <v>1</v>
+      </c>
+      <c r="T63" s="8">
+        <v>1</v>
+      </c>
+      <c r="U63" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D64" s="8"/>
+      <c r="F64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="U64" s="9"/>
+    </row>
+    <row r="65" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="8">
+        <v>1</v>
+      </c>
+      <c r="E65" s="8">
+        <v>1</v>
+      </c>
+      <c r="F65" s="8">
+        <v>1</v>
+      </c>
+      <c r="G65" s="8">
+        <v>1</v>
+      </c>
+      <c r="H65" s="8">
+        <v>1</v>
+      </c>
+      <c r="I65" s="8">
+        <v>1</v>
+      </c>
+      <c r="J65" s="8">
+        <v>1</v>
+      </c>
+      <c r="K65" s="8">
+        <v>1</v>
+      </c>
+      <c r="L65" s="8">
+        <v>1</v>
+      </c>
+      <c r="M65" s="8">
+        <v>1</v>
+      </c>
+      <c r="N65" s="8">
+        <v>1</v>
+      </c>
+      <c r="O65" s="8">
+        <v>1</v>
+      </c>
+      <c r="P65" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="8">
+        <v>1</v>
+      </c>
+      <c r="R65" s="8">
+        <v>1</v>
+      </c>
+      <c r="S65" s="8">
+        <v>1</v>
+      </c>
+      <c r="T65" s="8">
+        <v>1</v>
+      </c>
+      <c r="U65" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="8">
+        <v>1</v>
+      </c>
+      <c r="E66" s="8">
+        <v>1</v>
+      </c>
+      <c r="F66" s="8">
+        <v>1</v>
+      </c>
+      <c r="G66" s="8">
+        <v>1</v>
+      </c>
+      <c r="H66" s="8">
+        <v>1</v>
+      </c>
+      <c r="I66" s="8">
+        <v>1</v>
+      </c>
+      <c r="J66" s="8">
+        <v>1</v>
+      </c>
+      <c r="K66" s="8">
+        <v>1</v>
+      </c>
+      <c r="L66" s="8">
+        <v>1</v>
+      </c>
+      <c r="M66" s="8">
+        <v>1</v>
+      </c>
+      <c r="N66" s="8">
+        <v>1</v>
+      </c>
+      <c r="O66" s="8">
+        <v>1</v>
+      </c>
+      <c r="P66" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="8">
+        <v>1</v>
+      </c>
+      <c r="R66" s="8">
+        <v>1</v>
+      </c>
+      <c r="S66" s="8">
+        <v>1</v>
+      </c>
+      <c r="T66" s="8">
+        <v>1</v>
+      </c>
+      <c r="U66" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="D67" s="8"/>
+      <c r="F67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="R67" s="9"/>
+      <c r="U67" s="9"/>
+    </row>
+    <row r="68" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="8">
+        <v>1</v>
+      </c>
+      <c r="E68" s="8">
+        <v>1</v>
+      </c>
+      <c r="F68" s="8">
+        <v>1</v>
+      </c>
+      <c r="G68" s="8">
+        <v>1</v>
+      </c>
+      <c r="H68" s="8">
+        <v>1</v>
+      </c>
+      <c r="I68" s="8">
+        <v>1</v>
+      </c>
+      <c r="J68" s="8">
+        <v>1</v>
+      </c>
+      <c r="K68" s="8">
+        <v>1</v>
+      </c>
+      <c r="L68" s="8">
+        <v>1</v>
+      </c>
+      <c r="M68" s="8">
+        <v>1</v>
+      </c>
+      <c r="N68" s="8">
+        <v>1</v>
+      </c>
+      <c r="O68" s="8">
+        <v>1</v>
+      </c>
+      <c r="P68" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="8">
+        <v>1</v>
+      </c>
+      <c r="R68" s="8">
+        <v>1</v>
+      </c>
+      <c r="S68" s="8">
+        <v>1</v>
+      </c>
+      <c r="T68" s="8">
+        <v>1</v>
+      </c>
+      <c r="U68" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="D69" s="8">
+        <v>1</v>
+      </c>
+      <c r="E69" s="8">
+        <v>1</v>
+      </c>
+      <c r="F69" s="8">
+        <v>1</v>
+      </c>
+      <c r="G69" s="8">
+        <v>1</v>
+      </c>
+      <c r="H69" s="8">
+        <v>1</v>
+      </c>
+      <c r="I69" s="8">
+        <v>1</v>
+      </c>
+      <c r="J69" s="8">
+        <v>1</v>
+      </c>
+      <c r="K69" s="8">
+        <v>1</v>
+      </c>
+      <c r="L69" s="8">
+        <v>1</v>
+      </c>
+      <c r="M69" s="8">
+        <v>1</v>
+      </c>
+      <c r="N69" s="8">
+        <v>1</v>
+      </c>
+      <c r="O69" s="8">
+        <v>1</v>
+      </c>
+      <c r="P69" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="8">
+        <v>1</v>
+      </c>
+      <c r="R69" s="8">
+        <v>1</v>
+      </c>
+      <c r="S69" s="8">
+        <v>1</v>
+      </c>
+      <c r="T69" s="8">
+        <v>1</v>
+      </c>
+      <c r="U69" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C70" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AA21861009F844A94D45FCCECE366B4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e658606205e1dbc8e3f5b77287602906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c03d4cec-2a4e-42ae-b684-cd712438aa88" xmlns:ns4="8e23d785-2c7b-4ebd-b19b-adb2653ad200" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7ada76741c526a1ec7a93ee9c23d7ee" ns3:_="" ns4:_="">
     <xsd:import namespace="c03d4cec-2a4e-42ae-b684-cd712438aa88"/>
@@ -1920,24 +4765,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18DBFE82-80C8-4376-B234-6C09CB739632}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69518AF9-9CB4-408D-86CF-D237C82EA94C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1954,4 +4797,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18DBFE82-80C8-4376-B234-6C09CB739632}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed some formatting things with tables with rounding and nulls. Fixed table bugs. Converted table format to be two separate tables instead of one.
</commit_message>
<xml_diff>
--- a/Decoupling/tableTemplate.xlsx
+++ b/Decoupling/tableTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ensxvd_mail_missouri_edu/Documents/FAPRI/MarketResearch/Decoupling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="114_{E64F9D53-B268-47B0-A535-E4631D69459A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E620348-5AF6-472D-8203-6CC464F221A7}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="114_{E64F9D53-B268-47B0-A535-E4631D69459A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{851D2438-16AE-4435-A03F-EF7CE432C02C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2C021E1E-A2C6-47E3-A832-2AA0528880E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="104">
   <si>
     <t>Other</t>
   </si>
@@ -1945,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CFEF19-65F2-4B7A-B20C-D8F1581CCEE7}">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4811,6 +4811,9 @@
     <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>102</v>
+      </c>
+      <c r="D71" t="s">
+        <v>41</v>
       </c>
       <c r="E71" s="8">
         <v>1</v>
@@ -5100,18 +5103,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5134,18 +5137,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18DBFE82-80C8-4376-B234-6C09CB739632}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>